<commit_message>
Module maper screen design
</commit_message>
<xml_diff>
--- a/Android Assignment Task Matrix.xlsx
+++ b/Android Assignment Task Matrix.xlsx
@@ -3,13 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290EF3D5-A546-466F-AC84-C6C65128F803}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF79CD-4D38-41A2-9C90-212FE16390FA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$26</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="41">
   <si>
     <t>Start Date</t>
   </si>
@@ -132,9 +135,6 @@
     <t>Module edit Screen design and working</t>
   </si>
   <si>
-    <t>Sourabh sing</t>
-  </si>
-  <si>
     <t>Module Oberview Screen working and design</t>
   </si>
   <si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Assignments Screen design and working</t>
+  </si>
+  <si>
+    <t>Insert statement for Module</t>
   </si>
 </sst>
 </file>
@@ -466,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -741,39 +744,48 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>35</v>
       </c>
-      <c r="D22" t="s">
-        <v>36</v>
+      <c r="D22" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
         <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E26" xr:uid="{1764799F-DD9D-48C9-B7D4-2EA9F998AB6A}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>